<commit_message>
add DFT in matlab
</commit_message>
<xml_diff>
--- a/docs/rot_coef.xlsx
+++ b/docs/rot_coef.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -526,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S514"/>
+  <dimension ref="A1:U514"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U49" sqref="U49"/>
+    <sheetView tabSelected="1" topLeftCell="E191" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2:U227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,7 +542,7 @@
     <col min="14" max="14" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -580,7 +580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <f>COS(2*PI()*E2/$E$1)</f>
         <v>1</v>
@@ -630,8 +630,11 @@
       <c r="S2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <f t="shared" ref="A3:A17" si="1">COS(2*PI()*E3/$E$1)</f>
         <v>0.92387953251128674</v>
@@ -668,8 +671,11 @@
       </c>
       <c r="P3" s="20"/>
       <c r="Q3" s="22"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <f t="shared" si="1"/>
         <v>0.70710678118654757</v>
@@ -706,8 +712,11 @@
       </c>
       <c r="P4" s="20"/>
       <c r="Q4" s="22"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <f t="shared" si="1"/>
         <v>0.38268343236508984</v>
@@ -744,8 +753,11 @@
       </c>
       <c r="P5" s="20"/>
       <c r="Q5" s="22"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <f t="shared" si="1"/>
         <v>6.1257422745431001E-17</v>
@@ -787,8 +799,11 @@
       <c r="R6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <f t="shared" si="1"/>
         <v>-0.38268343236508973</v>
@@ -825,8 +840,11 @@
       </c>
       <c r="P7" s="20"/>
       <c r="Q7" s="22"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <f t="shared" si="1"/>
         <v>-0.70710678118654746</v>
@@ -863,8 +881,11 @@
       </c>
       <c r="P8" s="20"/>
       <c r="Q8" s="22"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <f t="shared" si="1"/>
         <v>-0.92387953251128674</v>
@@ -901,8 +922,11 @@
       </c>
       <c r="P9" s="20"/>
       <c r="Q9" s="22"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <f t="shared" si="1"/>
         <v>-1</v>
@@ -949,8 +973,11 @@
       <c r="R10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <f t="shared" si="1"/>
         <v>-0.92387953251128685</v>
@@ -992,8 +1019,11 @@
       </c>
       <c r="P11" s="20"/>
       <c r="Q11" s="22"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <f t="shared" si="1"/>
         <v>-0.70710678118654768</v>
@@ -1035,8 +1065,11 @@
       </c>
       <c r="P12" s="20"/>
       <c r="Q12" s="22"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <f t="shared" si="1"/>
         <v>-0.38268343236509034</v>
@@ -1078,8 +1111,11 @@
       </c>
       <c r="P13" s="20"/>
       <c r="Q13" s="22"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <f t="shared" si="1"/>
         <v>-1.83772268236293E-16</v>
@@ -1126,8 +1162,11 @@
       <c r="R14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <f t="shared" si="1"/>
         <v>0.38268343236509</v>
@@ -1169,8 +1208,11 @@
       </c>
       <c r="P15" s="20"/>
       <c r="Q15" s="22"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <f t="shared" si="1"/>
         <v>0.70710678118654735</v>
@@ -1212,8 +1254,11 @@
       </c>
       <c r="P16" s="20"/>
       <c r="Q16" s="22"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <f t="shared" si="1"/>
         <v>0.92387953251128652</v>
@@ -1255,8 +1300,11 @@
       </c>
       <c r="P17" s="20"/>
       <c r="Q17" s="22"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <f t="shared" ref="A18:A81" si="6">COS(2*PI()*E18/$E$1)</f>
         <v>1</v>
@@ -1308,8 +1356,11 @@
       <c r="S18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <f t="shared" si="6"/>
         <v>0.92387953251128674</v>
@@ -1351,8 +1402,11 @@
       </c>
       <c r="P19" s="20"/>
       <c r="Q19" s="22"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <f t="shared" si="6"/>
         <v>0.70710678118654768</v>
@@ -1389,8 +1443,11 @@
       </c>
       <c r="P20" s="20"/>
       <c r="Q20" s="22"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <f t="shared" si="6"/>
         <v>0.38268343236509045</v>
@@ -1427,8 +1484,11 @@
       </c>
       <c r="P21" s="20"/>
       <c r="Q21" s="22"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <f t="shared" si="6"/>
         <v>3.06287113727155E-16</v>
@@ -1470,8 +1530,11 @@
       <c r="R22">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <f t="shared" si="6"/>
         <v>-0.38268343236508989</v>
@@ -1508,8 +1571,11 @@
       </c>
       <c r="P23" s="20"/>
       <c r="Q23" s="22"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <f t="shared" si="6"/>
         <v>-0.70710678118654668</v>
@@ -1546,8 +1612,11 @@
       </c>
       <c r="P24" s="20"/>
       <c r="Q24" s="22"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <f t="shared" si="6"/>
         <v>-0.92387953251128641</v>
@@ -1584,8 +1653,11 @@
       </c>
       <c r="P25" s="20"/>
       <c r="Q25" s="22"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <f t="shared" si="6"/>
         <v>-1</v>
@@ -1627,8 +1699,11 @@
       <c r="R26">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <f t="shared" si="6"/>
         <v>-0.92387953251128674</v>
@@ -1665,8 +1740,11 @@
       </c>
       <c r="P27" s="20"/>
       <c r="Q27" s="22"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <f t="shared" si="6"/>
         <v>-0.70710678118654713</v>
@@ -1703,8 +1781,11 @@
       </c>
       <c r="P28" s="20"/>
       <c r="Q28" s="22"/>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <f t="shared" si="6"/>
         <v>-0.38268343236509056</v>
@@ -1741,8 +1822,11 @@
       </c>
       <c r="P29" s="20"/>
       <c r="Q29" s="22"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <f t="shared" si="6"/>
         <v>-4.28801959218017E-16</v>
@@ -1784,8 +1868,11 @@
       <c r="R30">
         <v>7</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U30">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <f t="shared" si="6"/>
         <v>0.38268343236508978</v>
@@ -1822,8 +1909,11 @@
       </c>
       <c r="P31" s="20"/>
       <c r="Q31" s="22"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <f t="shared" si="6"/>
         <v>0.70710678118654657</v>
@@ -1860,8 +1950,11 @@
       </c>
       <c r="P32" s="20"/>
       <c r="Q32" s="22"/>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <f t="shared" si="6"/>
         <v>0.92387953251128641</v>
@@ -1898,8 +1991,11 @@
       </c>
       <c r="P33" s="20"/>
       <c r="Q33" s="22"/>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U33">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <f t="shared" si="6"/>
         <v>1</v>
@@ -1946,8 +2042,11 @@
       <c r="S34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U34">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
         <f t="shared" si="6"/>
         <v>0.92387953251128674</v>
@@ -1984,8 +2083,11 @@
       </c>
       <c r="P35" s="20"/>
       <c r="Q35" s="22"/>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <f t="shared" si="6"/>
         <v>0.70710678118654724</v>
@@ -2022,8 +2124,11 @@
       </c>
       <c r="P36" s="20"/>
       <c r="Q36" s="22"/>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U36">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <f t="shared" si="6"/>
         <v>0.38268343236509067</v>
@@ -2060,8 +2165,11 @@
       </c>
       <c r="P37" s="20"/>
       <c r="Q37" s="22"/>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U37">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <f t="shared" si="6"/>
         <v>5.51316804708879E-16</v>
@@ -2103,8 +2211,11 @@
       <c r="R38">
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U38">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <f t="shared" si="6"/>
         <v>-0.38268343236508967</v>
@@ -2141,8 +2252,11 @@
       </c>
       <c r="P39" s="20"/>
       <c r="Q39" s="22"/>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U39">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <f t="shared" si="6"/>
         <v>-0.70710678118654646</v>
@@ -2179,8 +2293,11 @@
       </c>
       <c r="P40" s="20"/>
       <c r="Q40" s="22"/>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U40">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <f t="shared" si="6"/>
         <v>-0.92387953251128641</v>
@@ -2217,8 +2334,11 @@
       </c>
       <c r="P41" s="20"/>
       <c r="Q41" s="22"/>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U41">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <f t="shared" si="6"/>
         <v>-1</v>
@@ -2260,8 +2380,11 @@
       <c r="R42">
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U42">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <f t="shared" si="6"/>
         <v>-0.92387953251128752</v>
@@ -2298,8 +2421,11 @@
       </c>
       <c r="P43" s="20"/>
       <c r="Q43" s="22"/>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U43">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
         <f t="shared" si="6"/>
         <v>-0.70710678118654735</v>
@@ -2336,8 +2462,11 @@
       </c>
       <c r="P44" s="20"/>
       <c r="Q44" s="22"/>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U44">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
         <f t="shared" si="6"/>
         <v>-0.38268343236509078</v>
@@ -2374,8 +2503,11 @@
       </c>
       <c r="P45" s="20"/>
       <c r="Q45" s="22"/>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <f t="shared" si="6"/>
         <v>-2.4501884895999915E-15</v>
@@ -2417,8 +2549,11 @@
       <c r="R46">
         <v>11</v>
       </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U46">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <f t="shared" si="6"/>
         <v>0.38268343236508956</v>
@@ -2455,8 +2590,11 @@
       </c>
       <c r="P47" s="20"/>
       <c r="Q47" s="22"/>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U47">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
         <f t="shared" si="6"/>
         <v>0.70710678118654635</v>
@@ -2493,8 +2631,11 @@
       </c>
       <c r="P48" s="20"/>
       <c r="Q48" s="22"/>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U48">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
         <f t="shared" si="6"/>
         <v>0.92387953251128696</v>
@@ -2531,8 +2672,11 @@
       </c>
       <c r="P49" s="20"/>
       <c r="Q49" s="22"/>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U49">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
         <f t="shared" si="6"/>
         <v>1</v>
@@ -2579,8 +2723,11 @@
       <c r="S50">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U50">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
         <f t="shared" si="6"/>
         <v>0.92387953251128752</v>
@@ -2617,8 +2764,11 @@
       </c>
       <c r="P51" s="20"/>
       <c r="Q51" s="22"/>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U51">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
         <f t="shared" si="6"/>
         <v>0.70710678118654746</v>
@@ -2655,8 +2805,11 @@
       </c>
       <c r="P52" s="20"/>
       <c r="Q52" s="22"/>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
         <f t="shared" si="6"/>
         <v>0.38268343236509089</v>
@@ -2693,8 +2846,11 @@
       </c>
       <c r="P53" s="20"/>
       <c r="Q53" s="22"/>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U53">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
         <f t="shared" si="6"/>
         <v>-9.8001034370964746E-16</v>
@@ -2736,8 +2892,11 @@
       <c r="R54">
         <v>13</v>
       </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U54">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
         <f t="shared" si="6"/>
         <v>-0.38268343236508945</v>
@@ -2774,8 +2933,11 @@
       </c>
       <c r="P55" s="20"/>
       <c r="Q55" s="22"/>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U55">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
         <f t="shared" si="6"/>
         <v>-0.70710678118654635</v>
@@ -2812,8 +2974,11 @@
       </c>
       <c r="P56" s="20"/>
       <c r="Q56" s="22"/>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U56">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
         <f t="shared" si="6"/>
         <v>-0.92387953251128696</v>
@@ -2850,8 +3015,11 @@
       </c>
       <c r="P57" s="20"/>
       <c r="Q57" s="22"/>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U57">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="9">
         <f t="shared" si="6"/>
         <v>-1</v>
@@ -2893,8 +3061,11 @@
       <c r="R58">
         <v>14</v>
       </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U58">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="9">
         <f t="shared" si="6"/>
         <v>-0.92387953251128763</v>
@@ -2931,8 +3102,11 @@
       </c>
       <c r="P59" s="20"/>
       <c r="Q59" s="22"/>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U59">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="9">
         <f t="shared" si="6"/>
         <v>-0.70710678118654757</v>
@@ -2969,8 +3143,11 @@
       </c>
       <c r="P60" s="20"/>
       <c r="Q60" s="22"/>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U60">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="9">
         <f t="shared" si="6"/>
         <v>-0.382683432365091</v>
@@ -3007,8 +3184,11 @@
       </c>
       <c r="P61" s="20"/>
       <c r="Q61" s="22"/>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U61">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="9">
         <f t="shared" si="6"/>
         <v>-2.6952181805817155E-15</v>
@@ -3050,8 +3230,11 @@
       <c r="R62">
         <v>15</v>
       </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="9">
         <f t="shared" si="6"/>
         <v>0.38268343236508934</v>
@@ -3088,8 +3271,11 @@
       </c>
       <c r="P63" s="20"/>
       <c r="Q63" s="22"/>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U63">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
         <f t="shared" si="6"/>
         <v>0.70710678118654624</v>
@@ -3126,8 +3312,11 @@
       </c>
       <c r="P64" s="20"/>
       <c r="Q64" s="22"/>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U64">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="9">
         <f t="shared" si="6"/>
         <v>0.92387953251128685</v>
@@ -3163,8 +3352,11 @@
         <v>2037</v>
       </c>
       <c r="P65" s="20"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U65">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
         <f t="shared" si="6"/>
         <v>1</v>
@@ -3194,8 +3386,11 @@
       </c>
       <c r="M66" s="16"/>
       <c r="N66" s="16"/>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U66">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="9">
         <f t="shared" si="6"/>
         <v>0.92387953251128763</v>
@@ -3225,8 +3420,11 @@
       </c>
       <c r="M67" s="16"/>
       <c r="N67" s="16"/>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U67">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68" s="9">
         <f t="shared" si="6"/>
         <v>0.70710678118654757</v>
@@ -3256,8 +3454,11 @@
       </c>
       <c r="M68" s="16"/>
       <c r="N68" s="16"/>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U68">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="9">
         <f t="shared" si="6"/>
         <v>0.38268343236509111</v>
@@ -3287,8 +3488,11 @@
       </c>
       <c r="M69" s="16"/>
       <c r="N69" s="16"/>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U69">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" s="9">
         <f t="shared" si="6"/>
         <v>-7.3498065272792346E-16</v>
@@ -3318,8 +3522,11 @@
       </c>
       <c r="M70" s="16"/>
       <c r="N70" s="16"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U70">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" s="9">
         <f t="shared" si="6"/>
         <v>-0.38268343236508923</v>
@@ -3349,8 +3556,11 @@
       </c>
       <c r="M71" s="16"/>
       <c r="N71" s="16"/>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U71">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" s="9">
         <f t="shared" si="6"/>
         <v>-0.70710678118654613</v>
@@ -3380,8 +3590,11 @@
       </c>
       <c r="M72" s="16"/>
       <c r="N72" s="16"/>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U72">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" s="9">
         <f t="shared" si="6"/>
         <v>-0.92387953251128685</v>
@@ -3411,8 +3624,11 @@
       </c>
       <c r="M73" s="16"/>
       <c r="N73" s="16"/>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U73">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74" s="9">
         <f t="shared" si="6"/>
         <v>-1</v>
@@ -3442,8 +3658,11 @@
       </c>
       <c r="M74" s="16"/>
       <c r="N74" s="16"/>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U74">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A75" s="9">
         <f t="shared" si="6"/>
         <v>-0.92387953251128774</v>
@@ -3473,8 +3692,11 @@
       </c>
       <c r="M75" s="16"/>
       <c r="N75" s="16"/>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U75">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A76" s="9">
         <f t="shared" si="6"/>
         <v>-0.70710678118654768</v>
@@ -3504,8 +3726,11 @@
       </c>
       <c r="M76" s="16"/>
       <c r="N76" s="16"/>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U76">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A77" s="9">
         <f t="shared" si="6"/>
         <v>-0.38268343236509123</v>
@@ -3535,8 +3760,11 @@
       </c>
       <c r="M77" s="16"/>
       <c r="N77" s="16"/>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U77">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78" s="9">
         <f t="shared" si="6"/>
         <v>-2.9402478715634395E-15</v>
@@ -3566,8 +3794,11 @@
       </c>
       <c r="M78" s="16"/>
       <c r="N78" s="16"/>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U78">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A79" s="9">
         <f t="shared" si="6"/>
         <v>0.38268343236508912</v>
@@ -3597,8 +3828,11 @@
       </c>
       <c r="M79" s="16"/>
       <c r="N79" s="16"/>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U79">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" s="9">
         <f t="shared" si="6"/>
         <v>0.70710678118654602</v>
@@ -3628,8 +3862,11 @@
       </c>
       <c r="M80" s="16"/>
       <c r="N80" s="16"/>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U80">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81" s="9">
         <f t="shared" si="6"/>
         <v>0.92387953251128685</v>
@@ -3659,8 +3896,11 @@
       </c>
       <c r="M81" s="16"/>
       <c r="N81" s="16"/>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U81">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82" s="9">
         <f t="shared" ref="A82:A145" si="12">COS(2*PI()*E82/$E$1)</f>
         <v>1</v>
@@ -3690,8 +3930,11 @@
       </c>
       <c r="M82" s="16"/>
       <c r="N82" s="16"/>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U82">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83" s="9">
         <f t="shared" si="12"/>
         <v>0.92387953251128774</v>
@@ -3721,8 +3964,11 @@
       </c>
       <c r="M83" s="16"/>
       <c r="N83" s="16"/>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U83">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84" s="9">
         <f t="shared" si="12"/>
         <v>0.70710678118655035</v>
@@ -3752,8 +3998,11 @@
       </c>
       <c r="M84" s="16"/>
       <c r="N84" s="16"/>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U84">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85" s="9">
         <f t="shared" si="12"/>
         <v>0.38268343236508806</v>
@@ -3783,8 +4032,11 @@
       </c>
       <c r="M85" s="16"/>
       <c r="N85" s="16"/>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U85">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" s="9">
         <f t="shared" si="12"/>
         <v>-4.8995096174619945E-16</v>
@@ -3814,8 +4066,11 @@
       </c>
       <c r="M86" s="16"/>
       <c r="N86" s="16"/>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U86">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87" s="9">
         <f t="shared" si="12"/>
         <v>-0.382683432365089</v>
@@ -3845,8 +4100,11 @@
       </c>
       <c r="M87" s="16"/>
       <c r="N87" s="16"/>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U87">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88" s="9">
         <f t="shared" si="12"/>
         <v>-0.70710678118654602</v>
@@ -3876,8 +4134,11 @@
       </c>
       <c r="M88" s="16"/>
       <c r="N88" s="16"/>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U88">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
         <f t="shared" si="12"/>
         <v>-0.92387953251128541</v>
@@ -3907,8 +4168,11 @@
       </c>
       <c r="M89" s="16"/>
       <c r="N89" s="16"/>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U89">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
         <f t="shared" si="12"/>
         <v>-1</v>
@@ -3938,8 +4202,11 @@
       </c>
       <c r="M90" s="16"/>
       <c r="N90" s="16"/>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U90">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91" s="9">
         <f t="shared" si="12"/>
         <v>-0.92387953251128641</v>
@@ -3969,8 +4236,11 @@
       </c>
       <c r="M91" s="16"/>
       <c r="N91" s="16"/>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U91">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92" s="9">
         <f t="shared" si="12"/>
         <v>-0.70710678118654791</v>
@@ -4000,8 +4270,11 @@
       </c>
       <c r="M92" s="16"/>
       <c r="N92" s="16"/>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U92">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93" s="9">
         <f t="shared" si="12"/>
         <v>-0.38268343236509145</v>
@@ -4031,8 +4304,11 @@
       </c>
       <c r="M93" s="16"/>
       <c r="N93" s="16"/>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U93">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94" s="9">
         <f t="shared" si="12"/>
         <v>-3.1852775625451635E-15</v>
@@ -4062,8 +4338,11 @@
       </c>
       <c r="M94" s="16"/>
       <c r="N94" s="16"/>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U94">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A95" s="9">
         <f t="shared" si="12"/>
         <v>0.38268343236508556</v>
@@ -4093,8 +4372,11 @@
       </c>
       <c r="M95" s="16"/>
       <c r="N95" s="16"/>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U95">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A96" s="9">
         <f t="shared" si="12"/>
         <v>0.70710678118654835</v>
@@ -4124,8 +4406,11 @@
       </c>
       <c r="M96" s="16"/>
       <c r="N96" s="16"/>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U96">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97" s="9">
         <f t="shared" si="12"/>
         <v>0.92387953251128674</v>
@@ -4155,8 +4440,11 @@
       </c>
       <c r="M97" s="16"/>
       <c r="N97" s="16"/>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U97">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A98" s="9">
         <f t="shared" si="12"/>
         <v>1</v>
@@ -4186,8 +4474,11 @@
       </c>
       <c r="M98" s="16"/>
       <c r="N98" s="16"/>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U98">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A99" s="9">
         <f t="shared" si="12"/>
         <v>0.92387953251128785</v>
@@ -4217,8 +4508,11 @@
       </c>
       <c r="M99" s="16"/>
       <c r="N99" s="16"/>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U99">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A100" s="9">
         <f t="shared" si="12"/>
         <v>0.70710678118655046</v>
@@ -4248,8 +4542,11 @@
       </c>
       <c r="M100" s="16"/>
       <c r="N100" s="16"/>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U100">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A101" s="9">
         <f t="shared" si="12"/>
         <v>0.38268343236508828</v>
@@ -4279,8 +4576,11 @@
       </c>
       <c r="M101" s="16"/>
       <c r="N101" s="16"/>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U101">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A102" s="9">
         <f t="shared" si="12"/>
         <v>-2.4492127076447545E-16</v>
@@ -4310,8 +4610,11 @@
       </c>
       <c r="M102" s="16"/>
       <c r="N102" s="16"/>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U102">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A103" s="9">
         <f t="shared" si="12"/>
         <v>-0.38268343236508873</v>
@@ -4341,8 +4644,11 @@
       </c>
       <c r="M103" s="16"/>
       <c r="N103" s="16"/>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U103">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A104" s="9">
         <f t="shared" si="12"/>
         <v>-0.7071067811865458</v>
@@ -4372,8 +4678,11 @@
       </c>
       <c r="M104" s="16"/>
       <c r="N104" s="16"/>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U104">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A105" s="9">
         <f t="shared" si="12"/>
         <v>-0.9238795325112853</v>
@@ -4403,8 +4712,11 @@
       </c>
       <c r="M105" s="16"/>
       <c r="N105" s="16"/>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U105">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A106" s="9">
         <f t="shared" si="12"/>
         <v>-1</v>
@@ -4434,8 +4746,11 @@
       </c>
       <c r="M106" s="16"/>
       <c r="N106" s="16"/>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U106">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A107" s="9">
         <f t="shared" si="12"/>
         <v>-0.92387953251128652</v>
@@ -4465,8 +4780,11 @@
       </c>
       <c r="M107" s="16"/>
       <c r="N107" s="16"/>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U107">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A108" s="9">
         <f t="shared" si="12"/>
         <v>-0.70710678118654802</v>
@@ -4496,8 +4814,11 @@
       </c>
       <c r="M108" s="16"/>
       <c r="N108" s="16"/>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U108">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A109" s="9">
         <f t="shared" si="12"/>
         <v>-0.38268343236509167</v>
@@ -4527,8 +4848,11 @@
       </c>
       <c r="M109" s="16"/>
       <c r="N109" s="16"/>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U109">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A110" s="9">
         <f t="shared" si="12"/>
         <v>-3.4303072535268875E-15</v>
@@ -4558,8 +4882,11 @@
       </c>
       <c r="M110" s="16"/>
       <c r="N110" s="16"/>
-    </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U110">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A111" s="9">
         <f t="shared" si="12"/>
         <v>0.38268343236508534</v>
@@ -4589,8 +4916,11 @@
       </c>
       <c r="M111" s="16"/>
       <c r="N111" s="16"/>
-    </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U111">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A112" s="9">
         <f t="shared" si="12"/>
         <v>0.70710678118654824</v>
@@ -4620,8 +4950,11 @@
       </c>
       <c r="M112" s="16"/>
       <c r="N112" s="16"/>
-    </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U112">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A113" s="9">
         <f t="shared" si="12"/>
         <v>0.92387953251128663</v>
@@ -4651,8 +4984,11 @@
       </c>
       <c r="M113" s="16"/>
       <c r="N113" s="16"/>
-    </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U113">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A114" s="9">
         <f t="shared" si="12"/>
         <v>1</v>
@@ -4682,8 +5018,11 @@
       </c>
       <c r="M114" s="16"/>
       <c r="N114" s="16"/>
-    </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U114">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A115" s="9">
         <f t="shared" si="12"/>
         <v>0.92387953251128796</v>
@@ -4713,8 +5052,11 @@
       </c>
       <c r="M115" s="16"/>
       <c r="N115" s="16"/>
-    </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U115">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A116" s="9">
         <f t="shared" si="12"/>
         <v>0.70710678118655068</v>
@@ -4744,8 +5086,11 @@
       </c>
       <c r="M116" s="16"/>
       <c r="N116" s="16"/>
-    </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U116">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A117" s="9">
         <f t="shared" si="12"/>
         <v>0.38268343236508851</v>
@@ -4775,8 +5120,11 @@
       </c>
       <c r="M117" s="16"/>
       <c r="N117" s="16"/>
-    </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U117">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A118" s="9">
         <f t="shared" si="12"/>
         <v>1.0842021724855044E-19</v>
@@ -4806,8 +5154,11 @@
       </c>
       <c r="M118" s="16"/>
       <c r="N118" s="16"/>
-    </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U118">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A119" s="9">
         <f t="shared" si="12"/>
         <v>-0.38268343236508851</v>
@@ -4837,8 +5188,11 @@
       </c>
       <c r="M119" s="16"/>
       <c r="N119" s="16"/>
-    </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U119">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A120" s="9">
         <f t="shared" si="12"/>
         <v>-0.70710678118654557</v>
@@ -4868,8 +5222,11 @@
       </c>
       <c r="M120" s="16"/>
       <c r="N120" s="16"/>
-    </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U120">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A121" s="9">
         <f t="shared" si="12"/>
         <v>-0.92387953251128518</v>
@@ -4899,8 +5256,11 @@
       </c>
       <c r="M121" s="16"/>
       <c r="N121" s="16"/>
-    </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U121">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="122" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A122" s="9">
         <f t="shared" si="12"/>
         <v>-1</v>
@@ -4930,8 +5290,11 @@
       </c>
       <c r="M122" s="16"/>
       <c r="N122" s="16"/>
-    </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U122">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="123" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A123" s="9">
         <f t="shared" si="12"/>
         <v>-0.92387953251128663</v>
@@ -4961,8 +5324,11 @@
       </c>
       <c r="M123" s="16"/>
       <c r="N123" s="16"/>
-    </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U123">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="124" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A124" s="9">
         <f t="shared" si="12"/>
         <v>-0.70710678118654824</v>
@@ -4992,8 +5358,11 @@
       </c>
       <c r="M124" s="16"/>
       <c r="N124" s="16"/>
-    </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U124">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="125" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A125" s="9">
         <f t="shared" si="12"/>
         <v>-0.38268343236509195</v>
@@ -5023,8 +5392,11 @@
       </c>
       <c r="M125" s="16"/>
       <c r="N125" s="16"/>
-    </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U125">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="126" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A126" s="9">
         <f t="shared" si="12"/>
         <v>-3.6753369445086115E-15</v>
@@ -5054,8 +5426,11 @@
       </c>
       <c r="M126" s="16"/>
       <c r="N126" s="16"/>
-    </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U126">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="127" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A127" s="9">
         <f t="shared" si="12"/>
         <v>0.38268343236508512</v>
@@ -5085,8 +5460,11 @@
       </c>
       <c r="M127" s="16"/>
       <c r="N127" s="16"/>
-    </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U127">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="128" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A128" s="9">
         <f t="shared" si="12"/>
         <v>0.70710678118654802</v>
@@ -5116,8 +5494,11 @@
       </c>
       <c r="M128" s="16"/>
       <c r="N128" s="16"/>
-    </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U128">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="129" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A129" s="9">
         <f t="shared" si="12"/>
         <v>0.92387953251128652</v>
@@ -5147,8 +5528,11 @@
       </c>
       <c r="M129" s="16"/>
       <c r="N129" s="16"/>
-    </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U129">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="130" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A130" s="9">
         <f t="shared" si="12"/>
         <v>1</v>
@@ -5178,8 +5562,11 @@
       </c>
       <c r="M130" s="16"/>
       <c r="N130" s="16"/>
-    </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U130">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="131" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A131" s="9">
         <f t="shared" si="12"/>
         <v>0.92387953251128807</v>
@@ -5209,8 +5596,11 @@
       </c>
       <c r="M131" s="16"/>
       <c r="N131" s="16"/>
-    </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U131">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="132" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A132" s="9">
         <f t="shared" si="12"/>
         <v>0.70710678118655079</v>
@@ -5240,8 +5630,11 @@
       </c>
       <c r="M132" s="16"/>
       <c r="N132" s="16"/>
-    </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U132">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="133" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A133" s="9">
         <f t="shared" si="12"/>
         <v>0.38268343236508873</v>
@@ -5271,8 +5664,11 @@
       </c>
       <c r="M133" s="16"/>
       <c r="N133" s="16"/>
-    </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U133">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="134" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A134" s="9">
         <f t="shared" si="12"/>
         <v>2.4513811119897255E-16</v>
@@ -5302,8 +5698,11 @@
       </c>
       <c r="M134" s="16"/>
       <c r="N134" s="16"/>
-    </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U134">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="135" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A135" s="9">
         <f t="shared" si="12"/>
         <v>-0.38268343236508828</v>
@@ -5333,8 +5732,11 @@
       </c>
       <c r="M135" s="16"/>
       <c r="N135" s="16"/>
-    </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U135">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="136" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A136" s="9">
         <f t="shared" si="12"/>
         <v>-0.70710678118654546</v>
@@ -5364,8 +5766,11 @@
       </c>
       <c r="M136" s="16"/>
       <c r="N136" s="16"/>
-    </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U136">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="137" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A137" s="9">
         <f t="shared" si="12"/>
         <v>-0.92387953251128507</v>
@@ -5395,8 +5800,11 @@
       </c>
       <c r="M137" s="16"/>
       <c r="N137" s="16"/>
-    </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U137">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="138" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A138" s="9">
         <f t="shared" si="12"/>
         <v>-1</v>
@@ -5426,8 +5834,11 @@
       </c>
       <c r="M138" s="16"/>
       <c r="N138" s="16"/>
-    </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U138">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="139" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A139" s="9">
         <f t="shared" si="12"/>
         <v>-0.92387953251128674</v>
@@ -5457,8 +5868,11 @@
       </c>
       <c r="M139" s="16"/>
       <c r="N139" s="16"/>
-    </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U139">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="140" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A140" s="9">
         <f t="shared" si="12"/>
         <v>-0.70710678118654835</v>
@@ -5488,8 +5902,11 @@
       </c>
       <c r="M140" s="16"/>
       <c r="N140" s="16"/>
-    </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U140">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="141" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A141" s="9">
         <f t="shared" si="12"/>
         <v>-0.38268343236509217</v>
@@ -5519,8 +5936,11 @@
       </c>
       <c r="M141" s="16"/>
       <c r="N141" s="16"/>
-    </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U141">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="142" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A142" s="9">
         <f t="shared" si="12"/>
         <v>-3.9203666354903355E-15</v>
@@ -5550,8 +5970,11 @@
       </c>
       <c r="M142" s="16"/>
       <c r="N142" s="16"/>
-    </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U142">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="143" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A143" s="9">
         <f t="shared" si="12"/>
         <v>0.3826834323650849</v>
@@ -5581,8 +6004,11 @@
       </c>
       <c r="M143" s="16"/>
       <c r="N143" s="16"/>
-    </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U143">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="144" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A144" s="9">
         <f t="shared" si="12"/>
         <v>0.70710678118654791</v>
@@ -5612,8 +6038,11 @@
       </c>
       <c r="M144" s="16"/>
       <c r="N144" s="16"/>
-    </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U144">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="145" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A145" s="9">
         <f t="shared" si="12"/>
         <v>0.92387953251128641</v>
@@ -5643,8 +6072,11 @@
       </c>
       <c r="M145" s="16"/>
       <c r="N145" s="16"/>
-    </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U145">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="146" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A146" s="9">
         <f t="shared" ref="A146:A209" si="19">COS(2*PI()*E146/$E$1)</f>
         <v>1</v>
@@ -5674,8 +6106,11 @@
       </c>
       <c r="M146" s="16"/>
       <c r="N146" s="16"/>
-    </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U146">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="147" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A147" s="9">
         <f t="shared" si="19"/>
         <v>0.92387953251128807</v>
@@ -5705,8 +6140,11 @@
       </c>
       <c r="M147" s="16"/>
       <c r="N147" s="16"/>
-    </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U147">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="148" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A148" s="9">
         <f t="shared" si="19"/>
         <v>0.70710678118655101</v>
@@ -5736,8 +6174,11 @@
       </c>
       <c r="M148" s="16"/>
       <c r="N148" s="16"/>
-    </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U148">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="149" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A149" s="9">
         <f t="shared" si="19"/>
         <v>0.382683432365089</v>
@@ -5767,8 +6208,11 @@
       </c>
       <c r="M149" s="16"/>
       <c r="N149" s="16"/>
-    </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U149">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="150" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A150" s="9">
         <f t="shared" si="19"/>
         <v>4.9016780218069655E-16</v>
@@ -5798,8 +6242,11 @@
       </c>
       <c r="M150" s="16"/>
       <c r="N150" s="16"/>
-    </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U150">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="151" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A151" s="9">
         <f t="shared" si="19"/>
         <v>-0.38268343236508806</v>
@@ -5829,8 +6276,11 @@
       </c>
       <c r="M151" s="16"/>
       <c r="N151" s="16"/>
-    </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U151">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="152" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A152" s="9">
         <f t="shared" si="19"/>
         <v>-0.70710678118654524</v>
@@ -5860,8 +6310,11 @@
       </c>
       <c r="M152" s="16"/>
       <c r="N152" s="16"/>
-    </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U152">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="153" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A153" s="9">
         <f t="shared" si="19"/>
         <v>-0.92387953251128507</v>
@@ -5891,8 +6344,11 @@
       </c>
       <c r="M153" s="16"/>
       <c r="N153" s="16"/>
-    </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U153">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="154" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A154" s="9">
         <f t="shared" si="19"/>
         <v>-1</v>
@@ -5922,8 +6378,11 @@
       </c>
       <c r="M154" s="16"/>
       <c r="N154" s="16"/>
-    </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U154">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="155" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A155" s="9">
         <f t="shared" si="19"/>
         <v>-0.92387953251128685</v>
@@ -5953,8 +6412,11 @@
       </c>
       <c r="M155" s="16"/>
       <c r="N155" s="16"/>
-    </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U155">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="156" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A156" s="9">
         <f t="shared" si="19"/>
         <v>-0.70710678118654857</v>
@@ -5984,8 +6446,11 @@
       </c>
       <c r="M156" s="16"/>
       <c r="N156" s="16"/>
-    </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U156">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="157" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A157" s="9">
         <f t="shared" si="19"/>
         <v>-0.38268343236509239</v>
@@ -6015,8 +6480,11 @@
       </c>
       <c r="M157" s="16"/>
       <c r="N157" s="16"/>
-    </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U157">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="158" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A158" s="9">
         <f t="shared" si="19"/>
         <v>-4.1653963264720595E-15</v>
@@ -6046,8 +6514,11 @@
       </c>
       <c r="M158" s="16"/>
       <c r="N158" s="16"/>
-    </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U158">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="159" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A159" s="9">
         <f t="shared" si="19"/>
         <v>0.38268343236508467</v>
@@ -6077,8 +6548,11 @@
       </c>
       <c r="M159" s="16"/>
       <c r="N159" s="16"/>
-    </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U159">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="160" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A160" s="9">
         <f t="shared" si="19"/>
         <v>0.70710678118654768</v>
@@ -6108,8 +6582,11 @@
       </c>
       <c r="M160" s="16"/>
       <c r="N160" s="16"/>
-    </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U160">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="161" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A161" s="9">
         <f t="shared" si="19"/>
         <v>0.92387953251128629</v>
@@ -6139,8 +6616,11 @@
       </c>
       <c r="M161" s="16"/>
       <c r="N161" s="16"/>
-    </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U161">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="162" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A162" s="9">
         <f t="shared" si="19"/>
         <v>1</v>
@@ -6170,8 +6650,11 @@
       </c>
       <c r="M162" s="16"/>
       <c r="N162" s="16"/>
-    </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U162">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="163" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A163" s="9">
         <f t="shared" si="19"/>
         <v>0.92387953251128818</v>
@@ -6201,8 +6684,11 @@
       </c>
       <c r="M163" s="16"/>
       <c r="N163" s="16"/>
-    </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U163">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="164" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A164" s="9">
         <f t="shared" si="19"/>
         <v>0.70710678118655113</v>
@@ -6232,8 +6718,11 @@
       </c>
       <c r="M164" s="16"/>
       <c r="N164" s="16"/>
-    </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U164">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="165" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A165" s="9">
         <f t="shared" si="19"/>
         <v>0.38268343236509578</v>
@@ -6263,8 +6752,11 @@
       </c>
       <c r="M165" s="16"/>
       <c r="N165" s="16"/>
-    </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U165">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="166" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A166" s="9">
         <f t="shared" si="19"/>
         <v>7.8406248507634224E-15</v>
@@ -6294,8 +6786,11 @@
       </c>
       <c r="M166" s="16"/>
       <c r="N166" s="16"/>
-    </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U166">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="167" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A167" s="9">
         <f t="shared" si="19"/>
         <v>-0.38268343236508129</v>
@@ -6325,8 +6820,11 @@
       </c>
       <c r="M167" s="16"/>
       <c r="N167" s="16"/>
-    </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U167">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="168" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A168" s="9">
         <f t="shared" si="19"/>
         <v>-0.70710678118655013</v>
@@ -6356,8 +6854,11 @@
       </c>
       <c r="M168" s="16"/>
       <c r="N168" s="16"/>
-    </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U168">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="169" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A169" s="9">
         <f t="shared" si="19"/>
         <v>-0.92387953251128763</v>
@@ -6387,8 +6888,11 @@
       </c>
       <c r="M169" s="16"/>
       <c r="N169" s="16"/>
-    </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U169">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="170" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A170" s="9">
         <f t="shared" si="19"/>
         <v>-1</v>
@@ -6418,8 +6922,11 @@
       </c>
       <c r="M170" s="16"/>
       <c r="N170" s="16"/>
-    </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U170">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="171" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A171" s="9">
         <f t="shared" si="19"/>
         <v>-0.92387953251128685</v>
@@ -6449,8 +6956,11 @@
       </c>
       <c r="M171" s="16"/>
       <c r="N171" s="16"/>
-    </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U171">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="172" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A172" s="9">
         <f t="shared" si="19"/>
         <v>-0.70710678118654868</v>
@@ -6480,8 +6990,11 @@
       </c>
       <c r="M172" s="16"/>
       <c r="N172" s="16"/>
-    </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U172">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="173" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A173" s="9">
         <f t="shared" si="19"/>
         <v>-0.38268343236509261</v>
@@ -6511,8 +7024,11 @@
       </c>
       <c r="M173" s="16"/>
       <c r="N173" s="16"/>
-    </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U173">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="174" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A174" s="9">
         <f t="shared" si="19"/>
         <v>-4.4104260174537835E-15</v>
@@ -6542,8 +7058,11 @@
       </c>
       <c r="M174" s="16"/>
       <c r="N174" s="16"/>
-    </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U174">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="175" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A175" s="9">
         <f t="shared" si="19"/>
         <v>0.38268343236508445</v>
@@ -6573,8 +7092,11 @@
       </c>
       <c r="M175" s="16"/>
       <c r="N175" s="16"/>
-    </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U175">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="176" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A176" s="9">
         <f t="shared" si="19"/>
         <v>0.70710678118654247</v>
@@ -6604,8 +7126,11 @@
       </c>
       <c r="M176" s="16"/>
       <c r="N176" s="16"/>
-    </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U176">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="177" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A177" s="9">
         <f t="shared" si="19"/>
         <v>0.92387953251128352</v>
@@ -6635,8 +7160,11 @@
       </c>
       <c r="M177" s="16"/>
       <c r="N177" s="16"/>
-    </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U177">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="178" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A178" s="9">
         <f t="shared" si="19"/>
         <v>1</v>
@@ -6666,8 +7194,11 @@
       </c>
       <c r="M178" s="16"/>
       <c r="N178" s="16"/>
-    </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U178">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="179" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A179" s="9">
         <f t="shared" si="19"/>
         <v>0.92387953251128563</v>
@@ -6697,8 +7228,11 @@
       </c>
       <c r="M179" s="16"/>
       <c r="N179" s="16"/>
-    </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U179">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="180" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A180" s="9">
         <f t="shared" si="19"/>
         <v>0.70710678118654635</v>
@@ -6728,8 +7262,11 @@
       </c>
       <c r="M180" s="16"/>
       <c r="N180" s="16"/>
-    </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U180">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="181" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A181" s="9">
         <f t="shared" si="19"/>
         <v>0.38268343236508945</v>
@@ -6759,8 +7296,11 @@
       </c>
       <c r="M181" s="16"/>
       <c r="N181" s="16"/>
-    </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U181">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="182" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A182" s="9">
         <f t="shared" si="19"/>
         <v>9.8022718414414456E-16</v>
@@ -6790,8 +7330,11 @@
       </c>
       <c r="M182" s="16"/>
       <c r="N182" s="16"/>
-    </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U182">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="183" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A183" s="9">
         <f t="shared" si="19"/>
         <v>-0.38268343236508762</v>
@@ -6821,8 +7364,11 @@
       </c>
       <c r="M183" s="16"/>
       <c r="N183" s="16"/>
-    </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U183">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="184" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A184" s="9">
         <f t="shared" si="19"/>
         <v>-0.70710678118654491</v>
@@ -6852,8 +7398,11 @@
       </c>
       <c r="M184" s="16"/>
       <c r="N184" s="16"/>
-    </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U184">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="185" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A185" s="9">
         <f t="shared" si="19"/>
         <v>-0.92387953251128485</v>
@@ -6883,8 +7432,11 @@
       </c>
       <c r="M185" s="16"/>
       <c r="N185" s="16"/>
-    </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U185">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="186" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A186" s="9">
         <f t="shared" si="19"/>
         <v>-1</v>
@@ -6914,8 +7466,11 @@
       </c>
       <c r="M186" s="16"/>
       <c r="N186" s="16"/>
-    </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U186">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="187" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A187" s="9">
         <f t="shared" si="19"/>
         <v>-0.92387953251128974</v>
@@ -6945,8 +7500,11 @@
       </c>
       <c r="M187" s="16"/>
       <c r="N187" s="16"/>
-    </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U187">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="188" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A188" s="9">
         <f t="shared" si="19"/>
         <v>-0.7071067811865539</v>
@@ -6976,8 +7534,11 @@
       </c>
       <c r="M188" s="16"/>
       <c r="N188" s="16"/>
-    </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U188">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="189" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A189" s="9">
         <f t="shared" si="19"/>
         <v>-0.38268343236508628</v>
@@ -7007,8 +7568,11 @@
       </c>
       <c r="M189" s="16"/>
       <c r="N189" s="16"/>
-    </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U189">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="190" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A190" s="9">
         <f t="shared" si="19"/>
         <v>2.4499716491654944E-15</v>
@@ -7038,8 +7602,11 @@
       </c>
       <c r="M190" s="16"/>
       <c r="N190" s="16"/>
-    </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U190">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="191" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A191" s="9">
         <f t="shared" si="19"/>
         <v>0.38268343236509078</v>
@@ -7069,8 +7636,11 @@
       </c>
       <c r="M191" s="16"/>
       <c r="N191" s="16"/>
-    </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U191">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="192" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A192" s="9">
         <f t="shared" si="19"/>
         <v>0.70710678118654735</v>
@@ -7100,8 +7670,11 @@
       </c>
       <c r="M192" s="16"/>
       <c r="N192" s="16"/>
-    </row>
-    <row r="193" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U192">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="193" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A193" s="9">
         <f t="shared" si="19"/>
         <v>0.92387953251128618</v>
@@ -7131,8 +7704,11 @@
       </c>
       <c r="M193" s="16"/>
       <c r="N193" s="16"/>
-    </row>
-    <row r="194" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U193">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="194" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A194" s="9">
         <f t="shared" si="19"/>
         <v>1</v>
@@ -7162,8 +7738,11 @@
       </c>
       <c r="M194" s="16"/>
       <c r="N194" s="16"/>
-    </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U194">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="195" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A195" s="9">
         <f t="shared" si="19"/>
         <v>0.9238795325112884</v>
@@ -7193,8 +7772,11 @@
       </c>
       <c r="M195" s="16"/>
       <c r="N195" s="16"/>
-    </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U195">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="196" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A196" s="9">
         <f t="shared" si="19"/>
         <v>0.70710678118655146</v>
@@ -7224,8 +7806,11 @@
       </c>
       <c r="M196" s="16"/>
       <c r="N196" s="16"/>
-    </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U196">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="197" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A197" s="9">
         <f t="shared" si="19"/>
         <v>0.38268343236509622</v>
@@ -7255,8 +7840,11 @@
       </c>
       <c r="M197" s="16"/>
       <c r="N197" s="16"/>
-    </row>
-    <row r="198" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U197">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="198" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A198" s="9">
         <f t="shared" si="19"/>
         <v>8.3306842327268704E-15</v>
@@ -7286,8 +7874,11 @@
       </c>
       <c r="M198" s="16"/>
       <c r="N198" s="16"/>
-    </row>
-    <row r="199" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U198">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="199" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A199" s="9">
         <f t="shared" si="19"/>
         <v>-0.38268343236508084</v>
@@ -7317,8 +7908,11 @@
       </c>
       <c r="M199" s="16"/>
       <c r="N199" s="16"/>
-    </row>
-    <row r="200" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U199">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="200" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A200" s="9">
         <f t="shared" si="19"/>
         <v>-0.70710678118654979</v>
@@ -7348,8 +7942,11 @@
       </c>
       <c r="M200" s="16"/>
       <c r="N200" s="16"/>
-    </row>
-    <row r="201" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U200">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="201" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A201" s="9">
         <f t="shared" si="19"/>
         <v>-0.9238795325112874</v>
@@ -7379,8 +7976,11 @@
       </c>
       <c r="M201" s="16"/>
       <c r="N201" s="16"/>
-    </row>
-    <row r="202" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U201">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="202" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A202" s="9">
         <f t="shared" si="19"/>
         <v>-1</v>
@@ -7410,8 +8010,11 @@
       </c>
       <c r="M202" s="16"/>
       <c r="N202" s="16"/>
-    </row>
-    <row r="203" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U202">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="203" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A203" s="9">
         <f t="shared" si="19"/>
         <v>-0.92387953251128707</v>
@@ -7441,8 +8044,11 @@
       </c>
       <c r="M203" s="16"/>
       <c r="N203" s="16"/>
-    </row>
-    <row r="204" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U203">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="204" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A204" s="9">
         <f t="shared" si="19"/>
         <v>-0.70710678118654913</v>
@@ -7472,8 +8078,11 @@
       </c>
       <c r="M204" s="16"/>
       <c r="N204" s="16"/>
-    </row>
-    <row r="205" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U204">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="205" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A205" s="9">
         <f t="shared" si="19"/>
         <v>-0.38268343236509306</v>
@@ -7503,8 +8112,11 @@
       </c>
       <c r="M205" s="16"/>
       <c r="N205" s="16"/>
-    </row>
-    <row r="206" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U205">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="206" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A206" s="9">
         <f t="shared" si="19"/>
         <v>-4.9004853994172315E-15</v>
@@ -7534,8 +8146,11 @@
       </c>
       <c r="M206" s="16"/>
       <c r="N206" s="16"/>
-    </row>
-    <row r="207" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U206">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="207" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A207" s="9">
         <f t="shared" si="19"/>
         <v>0.38268343236508401</v>
@@ -7565,8 +8180,11 @@
       </c>
       <c r="M207" s="16"/>
       <c r="N207" s="16"/>
-    </row>
-    <row r="208" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U207">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="208" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A208" s="9">
         <f t="shared" si="19"/>
         <v>0.70710678118654213</v>
@@ -7596,8 +8214,11 @@
       </c>
       <c r="M208" s="16"/>
       <c r="N208" s="16"/>
-    </row>
-    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U208">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="209" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A209" s="9">
         <f t="shared" si="19"/>
         <v>0.9238795325112833</v>
@@ -7627,8 +8248,11 @@
       </c>
       <c r="M209" s="16"/>
       <c r="N209" s="16"/>
-    </row>
-    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U209">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="210" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A210" s="9">
         <f t="shared" ref="A210:A273" si="25">COS(2*PI()*E210/$E$1)</f>
         <v>1</v>
@@ -7658,8 +8282,11 @@
       </c>
       <c r="M210" s="16"/>
       <c r="N210" s="16"/>
-    </row>
-    <row r="211" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U210">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="211" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A211" s="9">
         <f t="shared" si="25"/>
         <v>0.92387953251128574</v>
@@ -7689,8 +8316,11 @@
       </c>
       <c r="M211" s="16"/>
       <c r="N211" s="16"/>
-    </row>
-    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U211">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="212" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A212" s="9">
         <f t="shared" si="25"/>
         <v>0.70710678118654668</v>
@@ -7720,8 +8350,11 @@
       </c>
       <c r="M212" s="16"/>
       <c r="N212" s="16"/>
-    </row>
-    <row r="213" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U212">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="213" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A213" s="9">
         <f t="shared" si="25"/>
         <v>0.38268343236508989</v>
@@ -7751,8 +8384,11 @@
       </c>
       <c r="M213" s="16"/>
       <c r="N213" s="16"/>
-    </row>
-    <row r="214" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U213">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="214" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A214" s="9">
         <f t="shared" si="25"/>
         <v>1.4702865661075926E-15</v>
@@ -7782,8 +8418,11 @@
       </c>
       <c r="M214" s="16"/>
       <c r="N214" s="16"/>
-    </row>
-    <row r="215" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U214">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="215" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A215" s="9">
         <f t="shared" si="25"/>
         <v>-0.38268343236508717</v>
@@ -7813,8 +8452,11 @@
       </c>
       <c r="M215" s="16"/>
       <c r="N215" s="16"/>
-    </row>
-    <row r="216" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U215">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="216" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A216" s="9">
         <f t="shared" si="25"/>
         <v>-0.70710678118654458</v>
@@ -7844,8 +8486,11 @@
       </c>
       <c r="M216" s="16"/>
       <c r="N216" s="16"/>
-    </row>
-    <row r="217" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U216">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="217" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A217" s="9">
         <f t="shared" si="25"/>
         <v>-0.92387953251128463</v>
@@ -7875,8 +8520,11 @@
       </c>
       <c r="M217" s="16"/>
       <c r="N217" s="16"/>
-    </row>
-    <row r="218" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U217">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="218" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A218" s="9">
         <f t="shared" si="25"/>
         <v>-1</v>
@@ -7906,8 +8554,11 @@
       </c>
       <c r="M218" s="16"/>
       <c r="N218" s="16"/>
-    </row>
-    <row r="219" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U218">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="219" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A219" s="9">
         <f t="shared" si="25"/>
         <v>-0.92387953251128985</v>
@@ -7937,8 +8588,11 @@
       </c>
       <c r="M219" s="16"/>
       <c r="N219" s="16"/>
-    </row>
-    <row r="220" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U219">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="220" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A220" s="9">
         <f t="shared" si="25"/>
         <v>-0.70710678118655423</v>
@@ -7968,8 +8622,11 @@
       </c>
       <c r="M220" s="16"/>
       <c r="N220" s="16"/>
-    </row>
-    <row r="221" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U220">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="221" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A221" s="9">
         <f t="shared" si="25"/>
         <v>-0.38268343236508673</v>
@@ -7999,8 +8656,11 @@
       </c>
       <c r="M221" s="16"/>
       <c r="N221" s="16"/>
-    </row>
-    <row r="222" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U221">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="222" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A222" s="9">
         <f t="shared" si="25"/>
         <v>1.9599122672020464E-15</v>
@@ -8030,8 +8690,11 @@
       </c>
       <c r="M222" s="16"/>
       <c r="N222" s="16"/>
-    </row>
-    <row r="223" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U222">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="223" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A223" s="9">
         <f t="shared" si="25"/>
         <v>0.38268343236509034</v>
@@ -8061,8 +8724,11 @@
       </c>
       <c r="M223" s="16"/>
       <c r="N223" s="16"/>
-    </row>
-    <row r="224" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U223">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="224" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A224" s="9">
         <f t="shared" si="25"/>
         <v>0.70710678118654702</v>
@@ -8092,8 +8758,11 @@
       </c>
       <c r="M224" s="16"/>
       <c r="N224" s="16"/>
-    </row>
-    <row r="225" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U224">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="225" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A225" s="9">
         <f t="shared" si="25"/>
         <v>0.92387953251128596</v>
@@ -8123,8 +8792,11 @@
       </c>
       <c r="M225" s="16"/>
       <c r="N225" s="16"/>
-    </row>
-    <row r="226" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U225">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="226" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A226" s="9">
         <f t="shared" si="25"/>
         <v>1</v>
@@ -8154,8 +8826,11 @@
       </c>
       <c r="M226" s="16"/>
       <c r="N226" s="16"/>
-    </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U226">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="227" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A227" s="9">
         <f t="shared" si="25"/>
         <v>0.92387953251128863</v>
@@ -8185,8 +8860,11 @@
       </c>
       <c r="M227" s="16"/>
       <c r="N227" s="16"/>
-    </row>
-    <row r="228" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="U227">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="228" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A228" s="9">
         <f t="shared" si="25"/>
         <v>0.7071067811865519</v>
@@ -8217,7 +8895,7 @@
       <c r="M228" s="16"/>
       <c r="N228" s="16"/>
     </row>
-    <row r="229" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A229" s="9">
         <f t="shared" si="25"/>
         <v>0.38268343236509667</v>
@@ -8248,7 +8926,7 @@
       <c r="M229" s="16"/>
       <c r="N229" s="16"/>
     </row>
-    <row r="230" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A230" s="9">
         <f t="shared" si="25"/>
         <v>8.8207436146903184E-15</v>
@@ -8279,7 +8957,7 @@
       <c r="M230" s="16"/>
       <c r="N230" s="16"/>
     </row>
-    <row r="231" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A231" s="9">
         <f t="shared" si="25"/>
         <v>-0.3826834323650804</v>
@@ -8310,7 +8988,7 @@
       <c r="M231" s="16"/>
       <c r="N231" s="16"/>
     </row>
-    <row r="232" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A232" s="9">
         <f t="shared" si="25"/>
         <v>-0.70710678118654946</v>
@@ -8341,7 +9019,7 @@
       <c r="M232" s="16"/>
       <c r="N232" s="16"/>
     </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A233" s="9">
         <f t="shared" si="25"/>
         <v>-0.92387953251128729</v>
@@ -8372,7 +9050,7 @@
       <c r="M233" s="16"/>
       <c r="N233" s="16"/>
     </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A234" s="9">
         <f t="shared" si="25"/>
         <v>-1</v>
@@ -8403,7 +9081,7 @@
       <c r="M234" s="16"/>
       <c r="N234" s="16"/>
     </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A235" s="9">
         <f t="shared" si="25"/>
         <v>-0.92387953251128729</v>
@@ -8434,7 +9112,7 @@
       <c r="M235" s="16"/>
       <c r="N235" s="16"/>
     </row>
-    <row r="236" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A236" s="9">
         <f t="shared" si="25"/>
         <v>-0.70710678118654946</v>
@@ -8465,7 +9143,7 @@
       <c r="M236" s="16"/>
       <c r="N236" s="16"/>
     </row>
-    <row r="237" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A237" s="9">
         <f t="shared" si="25"/>
         <v>-0.3826834323650935</v>
@@ -8496,7 +9174,7 @@
       <c r="M237" s="16"/>
       <c r="N237" s="16"/>
     </row>
-    <row r="238" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A238" s="9">
         <f t="shared" si="25"/>
         <v>-5.3905447813806795E-15</v>
@@ -8527,7 +9205,7 @@
       <c r="M238" s="16"/>
       <c r="N238" s="16"/>
     </row>
-    <row r="239" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A239" s="9">
         <f t="shared" si="25"/>
         <v>0.38268343236508356</v>
@@ -8558,7 +9236,7 @@
       <c r="M239" s="16"/>
       <c r="N239" s="16"/>
     </row>
-    <row r="240" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A240" s="9">
         <f t="shared" si="25"/>
         <v>0.7071067811865418</v>

</xml_diff>